<commit_message>
test login with data provider
</commit_message>
<xml_diff>
--- a/com.freecrm/src/test/resources/test_data.xlsx
+++ b/com.freecrm/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.freecrm\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589B4B96-C40B-4E85-9F56-B149859E1EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F7A96D-793E-49C3-AFA1-6D6EA7815B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{212D3968-0E05-4AE2-9CEC-76A0DDE657D7}"/>
   </bookViews>
@@ -618,7 +618,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Test search contacts completed
</commit_message>
<xml_diff>
--- a/com.freecrm/src/test/resources/test_data.xlsx
+++ b/com.freecrm/src/test/resources/test_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.freecrm\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E8B1A2-7810-4DF6-812B-ACA7A2D086A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D1C080-1BB1-4583-BC80-B87176B6726F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{212D3968-0E05-4AE2-9CEC-76A0DDE657D7}"/>
+    <workbookView xWindow="3900" yWindow="696" windowWidth="17280" windowHeight="8880" xr2:uid="{212D3968-0E05-4AE2-9CEC-76A0DDE657D7}"/>
   </bookViews>
   <sheets>
     <sheet name="doSignIn" sheetId="1" r:id="rId1"/>
     <sheet name="dnu" sheetId="2" r:id="rId2"/>
     <sheet name="doAddContact" sheetId="3" r:id="rId3"/>
+    <sheet name="doFilterSearchInContacts" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
   <si>
     <t>password</t>
   </si>
@@ -230,6 +231,9 @@
   </si>
   <si>
     <t>Abc1987@</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -619,7 +623,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,4 +964,39 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B9805A-94BB-4E26-9C64-7436167C01B2}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test add new tasks completed
</commit_message>
<xml_diff>
--- a/com.freecrm/src/test/resources/test_data.xlsx
+++ b/com.freecrm/src/test/resources/test_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.freecrm\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D1C080-1BB1-4583-BC80-B87176B6726F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2DC8C1-6FD0-4512-84B2-22547DF393DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="696" windowWidth="17280" windowHeight="8880" xr2:uid="{212D3968-0E05-4AE2-9CEC-76A0DDE657D7}"/>
+    <workbookView xWindow="1260" yWindow="984" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{212D3968-0E05-4AE2-9CEC-76A0DDE657D7}"/>
   </bookViews>
   <sheets>
     <sheet name="doSignIn" sheetId="1" r:id="rId1"/>
-    <sheet name="dnu" sheetId="2" r:id="rId2"/>
-    <sheet name="doAddContact" sheetId="3" r:id="rId3"/>
-    <sheet name="doFilterSearchInContacts" sheetId="4" r:id="rId4"/>
+    <sheet name="doAddTasks" sheetId="5" r:id="rId2"/>
+    <sheet name="dnu" sheetId="2" r:id="rId3"/>
+    <sheet name="doAddContact" sheetId="3" r:id="rId4"/>
+    <sheet name="doFilterSearchInContacts" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>password</t>
   </si>
@@ -234,6 +235,18 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Test add task1</t>
+  </si>
+  <si>
+    <t>Test add task2</t>
+  </si>
+  <si>
+    <t>Test add task3</t>
   </si>
 </sst>
 </file>
@@ -622,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4FF3B5-1BDB-4C2D-9C10-28134F46DDD4}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -671,6 +684,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D4F32A-B1AD-4121-9CAE-581F14AC8047}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7010E5-8B8E-411C-9FBC-B19075780DD4}">
   <dimension ref="A1:I23"/>
   <sheetViews>
@@ -823,7 +874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDA437D-FC17-45FC-9739-D1BE43334241}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -966,7 +1017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B9805A-94BB-4E26-9C64-7436167C01B2}">
   <dimension ref="A1:A4"/>
   <sheetViews>

</xml_diff>